<commit_message>
Added Codset project, switched project to CVX
</commit_message>
<xml_diff>
--- a/src/main/webapp/schedules/HepA.xlsx
+++ b/src/main/webapp/schedules/HepA.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\forecast\forecaster2012\schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\tch\forecaster\src\main\webapp\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595F930E-8C72-4006-B6A6-BD2AB7B3E480}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="405"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="405" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Schedules" sheetId="1" r:id="rId1"/>
-    <sheet name="XML" sheetId="2" r:id="rId2"/>
-    <sheet name="Test" sheetId="3" r:id="rId3"/>
+    <sheet name="Temp" sheetId="4" r:id="rId1"/>
+    <sheet name="Schedules" sheetId="1" r:id="rId2"/>
+    <sheet name="XML" sheetId="2" r:id="rId3"/>
+    <sheet name="Test" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$118</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Schedules!$A$1:$K$118</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="235">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -41,18 +51,12 @@
     <t>Vaccine</t>
   </si>
   <si>
-    <t>Trade Name(s)</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
     <t>Child</t>
   </si>
   <si>
-    <t>145, 1180, 1190, 1200</t>
-  </si>
-  <si>
     <t>Hep A</t>
   </si>
   <si>
@@ -69,9 +73,6 @@
   </si>
   <si>
     <t>Hep A, ped/adol, 3 dose</t>
-  </si>
-  <si>
-    <t>Hep A, pediatric, NOS</t>
   </si>
   <si>
     <t>Hep A-Hep B</t>
@@ -330,11 +331,479 @@
   <si>
     <t xml:space="preserve">Adult assumed to have completed Hep A series. </t>
   </si>
+  <si>
+    <t>TCH</t>
+  </si>
+  <si>
+    <t>CVX</t>
+  </si>
+  <si>
+    <t>CVX Label</t>
+  </si>
+  <si>
+    <t>DTaP</t>
+  </si>
+  <si>
+    <t>DTaP, 5 pertussis antigens</t>
+  </si>
+  <si>
+    <t>DTaP, unspecified formulation</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>DTP</t>
+  </si>
+  <si>
+    <t>DT (pediatric)</t>
+  </si>
+  <si>
+    <t>DTaP-Hib</t>
+  </si>
+  <si>
+    <t>DTaP-Hep B-IPV</t>
+  </si>
+  <si>
+    <t>DTaP-Hib-IPV</t>
+  </si>
+  <si>
+    <t>DTaP-IPV</t>
+  </si>
+  <si>
+    <t>DTP-Hib</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>Td (adult), adsorbed</t>
+  </si>
+  <si>
+    <t>Td (adult)</t>
+  </si>
+  <si>
+    <t>Td(adult) unspecified formulation</t>
+  </si>
+  <si>
+    <t>Tdap</t>
+  </si>
+  <si>
+    <t>Td (adult) preservative free</t>
+  </si>
+  <si>
+    <t>Hib, unspecified formulation</t>
+  </si>
+  <si>
+    <t>Hib-Hep B</t>
+  </si>
+  <si>
+    <t>Hep B, unspecified formulation</t>
+  </si>
+  <si>
+    <t>DTaP-IPV-HIB-HEP B, historical</t>
+  </si>
+  <si>
+    <t>DTaP,IPV,Hib,HepB</t>
+  </si>
+  <si>
+    <t>Hep A, pediatric, unspecified formulation</t>
+  </si>
+  <si>
+    <t>Hep A, unspecified formulation</t>
+  </si>
+  <si>
+    <t>IPV</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>OPV</t>
+  </si>
+  <si>
+    <t>polio, unspecified formulation</t>
+  </si>
+  <si>
+    <t>pneumococcal conjugate PCV 7</t>
+  </si>
+  <si>
+    <t>pneumococcal polysaccharide PPV23</t>
+  </si>
+  <si>
+    <t>pneumococcal, unspecified formulation</t>
+  </si>
+  <si>
+    <t>Pneumococcal Conjugate, unspecified formulation</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>MMR</t>
+  </si>
+  <si>
+    <t>MMRV</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>M/R</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>measles</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>mumps</t>
+  </si>
+  <si>
+    <t>meningococcal B, recombinant</t>
+  </si>
+  <si>
+    <t>meningococcal B, OMV</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>rubella</t>
+  </si>
+  <si>
+    <t>rubella/mumps</t>
+  </si>
+  <si>
+    <t>varicella</t>
+  </si>
+  <si>
+    <t>influenza, whole</t>
+  </si>
+  <si>
+    <t>influenza, unspecified formulation</t>
+  </si>
+  <si>
+    <t>influenza, recombinant, injectable, preservative free</t>
+  </si>
+  <si>
+    <t>Influenza, injectable,quadrivalent, preservative free, pediatric</t>
+  </si>
+  <si>
+    <t>influenza, live, intranasal</t>
+  </si>
+  <si>
+    <t>influenza, split (incl. purified surface antigen)</t>
+  </si>
+  <si>
+    <t>meningococcal MPSV4</t>
+  </si>
+  <si>
+    <t>meningococcal MCV4P</t>
+  </si>
+  <si>
+    <t>meningococcal, unspecified formulation</t>
+  </si>
+  <si>
+    <t>meningococcal MCV4, unspecified formulation</t>
+  </si>
+  <si>
+    <t>Influenza, high dose seasonal</t>
+  </si>
+  <si>
+    <t>Novel Influenza-H1N1-09, all formulations</t>
+  </si>
+  <si>
+    <t>Novel Influenza-H1N1-09, nasal</t>
+  </si>
+  <si>
+    <t>Novel influenza-H1N1-09, preservative-free</t>
+  </si>
+  <si>
+    <t>Novel influenza-H1N1-09</t>
+  </si>
+  <si>
+    <t>meningococcal C conjugate</t>
+  </si>
+  <si>
+    <t>Meningococcal MCV4O</t>
+  </si>
+  <si>
+    <t>Influenza, seasonal, injectable, preservative free</t>
+  </si>
+  <si>
+    <t>Influenza, seasonal, injectable</t>
+  </si>
+  <si>
+    <t>influenza, intradermal, quadrivalent, preservative free</t>
+  </si>
+  <si>
+    <t>influenza, seasonal, intradermal, preservative free</t>
+  </si>
+  <si>
+    <t>influenza, live, intranasal, quadrivalent</t>
+  </si>
+  <si>
+    <t>influenza nasal, unspecified formulation</t>
+  </si>
+  <si>
+    <t>influenza, injectable, quadrivalent, preservative free</t>
+  </si>
+  <si>
+    <t>influenza, injectable, quadrivalent</t>
+  </si>
+  <si>
+    <t>rotavirus, monovalent</t>
+  </si>
+  <si>
+    <t>rotavirus, pentavalent</t>
+  </si>
+  <si>
+    <t>rotavirus, tetravalent</t>
+  </si>
+  <si>
+    <t>Lyme disease</t>
+  </si>
+  <si>
+    <t>rabies, intramuscular injection</t>
+  </si>
+  <si>
+    <t>rabies, intradermal injection</t>
+  </si>
+  <si>
+    <t>rabies, unspecified formulation</t>
+  </si>
+  <si>
+    <t>BCG</t>
+  </si>
+  <si>
+    <t>rotavirus, unspecified formulation</t>
+  </si>
+  <si>
+    <t>Meningococcal C/Y-HIB PRP</t>
+  </si>
+  <si>
+    <t>HPV9</t>
+  </si>
+  <si>
+    <t>HPV, quadrivalent</t>
+  </si>
+  <si>
+    <t>HPV, bivalent</t>
+  </si>
+  <si>
+    <t>HPV, unspecified formulation</t>
+  </si>
+  <si>
+    <t>adenovirus, type 4</t>
+  </si>
+  <si>
+    <t>adenovirus, type 7</t>
+  </si>
+  <si>
+    <t>adenovirus, unspecified formulation</t>
+  </si>
+  <si>
+    <t>anthrax</t>
+  </si>
+  <si>
+    <t>botulinum antitoxin</t>
+  </si>
+  <si>
+    <t>cholera</t>
+  </si>
+  <si>
+    <t>CMVIG</t>
+  </si>
+  <si>
+    <t>dengue fever</t>
+  </si>
+  <si>
+    <t>diphtheria antitoxin</t>
+  </si>
+  <si>
+    <t>DTP-Hib-Hep B</t>
+  </si>
+  <si>
+    <t>hantavirus</t>
+  </si>
+  <si>
+    <t>HBIG</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>Hep B, adolescent or pediatric</t>
+  </si>
+  <si>
+    <t>Hep B, adolescent/high risk infant</t>
+  </si>
+  <si>
+    <t>Hep B, adult</t>
+  </si>
+  <si>
+    <t>Hep B, dialysis</t>
+  </si>
+  <si>
+    <t>Hep E</t>
+  </si>
+  <si>
+    <t>herpes simplex 2</t>
+  </si>
+  <si>
+    <t>Hib (PRP-D)</t>
+  </si>
+  <si>
+    <t>Hib (HbOC)</t>
+  </si>
+  <si>
+    <t>Hib (PRP-T)</t>
+  </si>
+  <si>
+    <t>Hib (PRP-OMP)</t>
+  </si>
+  <si>
+    <t>IG</t>
+  </si>
+  <si>
+    <t>IGIV</t>
+  </si>
+  <si>
+    <t>IG, unspecified formulation</t>
+  </si>
+  <si>
+    <t>Japanese encephalitis SC</t>
+  </si>
+  <si>
+    <t>Japanese Encephalitis IM</t>
+  </si>
+  <si>
+    <t>leishmaniasis</t>
+  </si>
+  <si>
+    <t>leprosy</t>
+  </si>
+  <si>
+    <t>malaria</t>
+  </si>
+  <si>
+    <t>melanoma</t>
+  </si>
+  <si>
+    <t>parainfluenza-3</t>
+  </si>
+  <si>
+    <t>pertussis</t>
+  </si>
+  <si>
+    <t>plague</t>
+  </si>
+  <si>
+    <t>Q fever</t>
+  </si>
+  <si>
+    <t>rheumatic fever</t>
+  </si>
+  <si>
+    <t>Rift Valley fever</t>
+  </si>
+  <si>
+    <t>RIG</t>
+  </si>
+  <si>
+    <t>RSV-IGIV</t>
+  </si>
+  <si>
+    <t>RSV-MAb</t>
+  </si>
+  <si>
+    <t>vaccinia (smallpox)</t>
+  </si>
+  <si>
+    <t>Staphylococcus bacterio lysate</t>
+  </si>
+  <si>
+    <t>tetanus toxoid, adsorbed</t>
+  </si>
+  <si>
+    <t>tick-borne encephalitis</t>
+  </si>
+  <si>
+    <t>TIG</t>
+  </si>
+  <si>
+    <t>TST-OT tine test</t>
+  </si>
+  <si>
+    <t>TST-PPD intradermal</t>
+  </si>
+  <si>
+    <t>TST-PPD tine test</t>
+  </si>
+  <si>
+    <t>TST, unspecified formulation</t>
+  </si>
+  <si>
+    <t>tularemia vaccine</t>
+  </si>
+  <si>
+    <t>typhoid, oral</t>
+  </si>
+  <si>
+    <t>typhoid, parenteral</t>
+  </si>
+  <si>
+    <t>typhoid, parenteral, AKD (U.S. military)</t>
+  </si>
+  <si>
+    <t>typhoid, ViCPs</t>
+  </si>
+  <si>
+    <t>typhoid, unspecified formulation</t>
+  </si>
+  <si>
+    <t>vaccinia immune globulin</t>
+  </si>
+  <si>
+    <t>VEE, inactivated</t>
+  </si>
+  <si>
+    <t>VEE, live</t>
+  </si>
+  <si>
+    <t>VEE, unspecified formulation</t>
+  </si>
+  <si>
+    <t>VZIG</t>
+  </si>
+  <si>
+    <t>yellow fever</t>
+  </si>
+  <si>
+    <t>zoster</t>
+  </si>
+  <si>
+    <t>typhus, historical</t>
+  </si>
+  <si>
+    <t>Pneumococcal conjugate PCV 13</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>31, 83, 84, 85</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
@@ -401,7 +870,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,6 +911,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="44"/>
         <bgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="26"/>
       </patternFill>
     </fill>
   </fills>
@@ -522,7 +997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -616,6 +1091,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -720,7 +1207,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1036" name="Picture 2"/>
+        <xdr:cNvPr id="1036" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1132,11 +1625,1681 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J117"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25648720-0CFB-4092-A441-D2BD1B8C03D5}">
+  <dimension ref="A1:C150"/>
+  <sheetViews>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>110</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>110</v>
+      </c>
+      <c r="B3">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>110</v>
+      </c>
+      <c r="B4">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>111</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>112</v>
+      </c>
+      <c r="B6">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>113</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>114</v>
+      </c>
+      <c r="B8">
+        <v>110</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>115</v>
+      </c>
+      <c r="B9">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>116</v>
+      </c>
+      <c r="B10">
+        <v>130</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>121</v>
+      </c>
+      <c r="B11">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>122</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>122</v>
+      </c>
+      <c r="B13">
+        <v>138</v>
+      </c>
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>122</v>
+      </c>
+      <c r="B14">
+        <v>139</v>
+      </c>
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>123</v>
+      </c>
+      <c r="B15">
+        <v>115</v>
+      </c>
+      <c r="C15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>124</v>
+      </c>
+      <c r="B16">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>128</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>136</v>
+      </c>
+      <c r="B18">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>137</v>
+      </c>
+      <c r="B19">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>142</v>
+      </c>
+      <c r="B20">
+        <v>132</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>142</v>
+      </c>
+      <c r="B21">
+        <v>146</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>145</v>
+      </c>
+      <c r="B22">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>145</v>
+      </c>
+      <c r="B23">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>146</v>
+      </c>
+      <c r="B24">
+        <v>104</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>147</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>148</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>153</v>
+      </c>
+      <c r="B27">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>154</v>
+      </c>
+      <c r="B28">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>155</v>
+      </c>
+      <c r="B29">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>156</v>
+      </c>
+      <c r="B30">
+        <v>109</v>
+      </c>
+      <c r="C30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>156</v>
+      </c>
+      <c r="B31">
+        <v>152</v>
+      </c>
+      <c r="C31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>158</v>
+      </c>
+      <c r="B32" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>159</v>
+      </c>
+      <c r="B33">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>160</v>
+      </c>
+      <c r="B34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>161</v>
+      </c>
+      <c r="B35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>162</v>
+      </c>
+      <c r="B36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>162</v>
+      </c>
+      <c r="B37">
+        <v>215</v>
+      </c>
+      <c r="C37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>163</v>
+      </c>
+      <c r="B38">
+        <v>216</v>
+      </c>
+      <c r="C38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>171</v>
+      </c>
+      <c r="B39" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>175</v>
+      </c>
+      <c r="B40">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>178</v>
+      </c>
+      <c r="B41">
+        <v>21</v>
+      </c>
+      <c r="C41" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>179</v>
+      </c>
+      <c r="B42">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>179</v>
+      </c>
+      <c r="B43">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>179</v>
+      </c>
+      <c r="B44">
+        <v>155</v>
+      </c>
+      <c r="C44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>179</v>
+      </c>
+      <c r="B45">
+        <v>161</v>
+      </c>
+      <c r="C45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>180</v>
+      </c>
+      <c r="B46">
+        <v>111</v>
+      </c>
+      <c r="C46" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>181</v>
+      </c>
+      <c r="B47">
+        <v>15</v>
+      </c>
+      <c r="C47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>182</v>
+      </c>
+      <c r="B48">
+        <v>32</v>
+      </c>
+      <c r="C48" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>183</v>
+      </c>
+      <c r="B49">
+        <v>114</v>
+      </c>
+      <c r="C49" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>184</v>
+      </c>
+      <c r="B50">
+        <v>108</v>
+      </c>
+      <c r="C50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>184</v>
+      </c>
+      <c r="B51">
+        <v>147</v>
+      </c>
+      <c r="C51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>185</v>
+      </c>
+      <c r="B52">
+        <v>135</v>
+      </c>
+      <c r="C52" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>186</v>
+      </c>
+      <c r="B53">
+        <v>128</v>
+      </c>
+      <c r="C53" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>187</v>
+      </c>
+      <c r="B54">
+        <v>125</v>
+      </c>
+      <c r="C54" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>188</v>
+      </c>
+      <c r="B55">
+        <v>126</v>
+      </c>
+      <c r="C55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>189</v>
+      </c>
+      <c r="B56">
+        <v>127</v>
+      </c>
+      <c r="C56" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>197</v>
+      </c>
+      <c r="B57">
+        <v>103</v>
+      </c>
+      <c r="C57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>198</v>
+      </c>
+      <c r="B58">
+        <v>136</v>
+      </c>
+      <c r="C58" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>200</v>
+      </c>
+      <c r="B59">
+        <v>140</v>
+      </c>
+      <c r="C59" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>201</v>
+      </c>
+      <c r="B60">
+        <v>141</v>
+      </c>
+      <c r="C60" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>202</v>
+      </c>
+      <c r="B61">
+        <v>166</v>
+      </c>
+      <c r="C61" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>202</v>
+      </c>
+      <c r="B62">
+        <v>144</v>
+      </c>
+      <c r="C62" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>203</v>
+      </c>
+      <c r="B63">
+        <v>149</v>
+      </c>
+      <c r="C63" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>203</v>
+      </c>
+      <c r="B64">
+        <v>151</v>
+      </c>
+      <c r="C64" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>204</v>
+      </c>
+      <c r="B65">
+        <v>150</v>
+      </c>
+      <c r="C65" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>204</v>
+      </c>
+      <c r="B66">
+        <v>158</v>
+      </c>
+      <c r="C66" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>206</v>
+      </c>
+      <c r="B67">
+        <v>119</v>
+      </c>
+      <c r="C67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>207</v>
+      </c>
+      <c r="B68">
+        <v>116</v>
+      </c>
+      <c r="C68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>208</v>
+      </c>
+      <c r="B69">
+        <v>74</v>
+      </c>
+      <c r="C69" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>209</v>
+      </c>
+      <c r="B70">
+        <v>66</v>
+      </c>
+      <c r="C70" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>210</v>
+      </c>
+      <c r="B71">
+        <v>18</v>
+      </c>
+      <c r="C71" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>210</v>
+      </c>
+      <c r="B72">
+        <v>40</v>
+      </c>
+      <c r="C72" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>210</v>
+      </c>
+      <c r="B73">
+        <v>90</v>
+      </c>
+      <c r="C73" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>211</v>
+      </c>
+      <c r="B74">
+        <v>19</v>
+      </c>
+      <c r="C74" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>212</v>
+      </c>
+      <c r="B75">
+        <v>122</v>
+      </c>
+      <c r="C75" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>213</v>
+      </c>
+      <c r="B76">
+        <v>148</v>
+      </c>
+      <c r="C76" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>214</v>
+      </c>
+      <c r="B77">
+        <v>165</v>
+      </c>
+      <c r="C77" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>215</v>
+      </c>
+      <c r="B78">
+        <v>162</v>
+      </c>
+      <c r="C78" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>216</v>
+      </c>
+      <c r="B79">
+        <v>163</v>
+      </c>
+      <c r="C79" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>390</v>
+      </c>
+      <c r="B80">
+        <v>62</v>
+      </c>
+      <c r="C80" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>391</v>
+      </c>
+      <c r="B81">
+        <v>118</v>
+      </c>
+      <c r="C81" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>391</v>
+      </c>
+      <c r="B82">
+        <v>137</v>
+      </c>
+      <c r="C82" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1000</v>
+      </c>
+      <c r="B83">
+        <v>54</v>
+      </c>
+      <c r="C83" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>1010</v>
+      </c>
+      <c r="B84">
+        <v>55</v>
+      </c>
+      <c r="C84" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>1020</v>
+      </c>
+      <c r="B85">
+        <v>82</v>
+      </c>
+      <c r="C85" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1030</v>
+      </c>
+      <c r="B86">
+        <v>24</v>
+      </c>
+      <c r="C86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>1050</v>
+      </c>
+      <c r="B87">
+        <v>27</v>
+      </c>
+      <c r="C87" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>1060</v>
+      </c>
+      <c r="B88">
+        <v>26</v>
+      </c>
+      <c r="C88" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>1070</v>
+      </c>
+      <c r="B89">
+        <v>29</v>
+      </c>
+      <c r="C89" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>1080</v>
+      </c>
+      <c r="B90">
+        <v>56</v>
+      </c>
+      <c r="C90" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>1090</v>
+      </c>
+      <c r="B91">
+        <v>12</v>
+      </c>
+      <c r="C91" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1150</v>
+      </c>
+      <c r="B92">
+        <v>102</v>
+      </c>
+      <c r="C92" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>1160</v>
+      </c>
+      <c r="B93">
+        <v>57</v>
+      </c>
+      <c r="C93" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>1170</v>
+      </c>
+      <c r="B94">
+        <v>52</v>
+      </c>
+      <c r="C94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>1180</v>
+      </c>
+      <c r="B95">
+        <v>83</v>
+      </c>
+      <c r="C95" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>1190</v>
+      </c>
+      <c r="B96">
+        <v>84</v>
+      </c>
+      <c r="C96" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>1230</v>
+      </c>
+      <c r="B97">
+        <v>30</v>
+      </c>
+      <c r="C97" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>1240</v>
+      </c>
+      <c r="B98" t="s">
+        <v>180</v>
+      </c>
+      <c r="C98" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>1250</v>
+      </c>
+      <c r="B99">
+        <v>42</v>
+      </c>
+      <c r="C99" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>1260</v>
+      </c>
+      <c r="B100">
+        <v>43</v>
+      </c>
+      <c r="C100" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>1270</v>
+      </c>
+      <c r="B101">
+        <v>44</v>
+      </c>
+      <c r="C101" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>1300</v>
+      </c>
+      <c r="B102">
+        <v>59</v>
+      </c>
+      <c r="C102" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>1310</v>
+      </c>
+      <c r="B103">
+        <v>60</v>
+      </c>
+      <c r="C103" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>1320</v>
+      </c>
+      <c r="B104">
+        <v>46</v>
+      </c>
+      <c r="C104" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>1330</v>
+      </c>
+      <c r="B105">
+        <v>47</v>
+      </c>
+      <c r="C105" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>1340</v>
+      </c>
+      <c r="B106">
+        <v>48</v>
+      </c>
+      <c r="C106" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>1350</v>
+      </c>
+      <c r="B107">
+        <v>49</v>
+      </c>
+      <c r="C107" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>1400</v>
+      </c>
+      <c r="B108">
+        <v>86</v>
+      </c>
+      <c r="C108" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>1410</v>
+      </c>
+      <c r="B109">
+        <v>87</v>
+      </c>
+      <c r="C109" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>1420</v>
+      </c>
+      <c r="B110">
+        <v>14</v>
+      </c>
+      <c r="C110" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>1490</v>
+      </c>
+      <c r="B111">
+        <v>39</v>
+      </c>
+      <c r="C111" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>1491</v>
+      </c>
+      <c r="B112">
+        <v>134</v>
+      </c>
+      <c r="C112" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>1510</v>
+      </c>
+      <c r="B113">
+        <v>64</v>
+      </c>
+      <c r="C113" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>1520</v>
+      </c>
+      <c r="B114">
+        <v>65</v>
+      </c>
+      <c r="C114" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>1570</v>
+      </c>
+      <c r="B115">
+        <v>67</v>
+      </c>
+      <c r="C115" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>1590</v>
+      </c>
+      <c r="B116">
+        <v>68</v>
+      </c>
+      <c r="C116" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>1630</v>
+      </c>
+      <c r="B117">
+        <v>69</v>
+      </c>
+      <c r="C117" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>1640</v>
+      </c>
+      <c r="B118">
+        <v>11</v>
+      </c>
+      <c r="C118" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>1650</v>
+      </c>
+      <c r="B119">
+        <v>23</v>
+      </c>
+      <c r="C119" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>1680</v>
+      </c>
+      <c r="B120">
+        <v>70</v>
+      </c>
+      <c r="C120" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>1720</v>
+      </c>
+      <c r="B121">
+        <v>72</v>
+      </c>
+      <c r="C121" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>1730</v>
+      </c>
+      <c r="B122">
+        <v>73</v>
+      </c>
+      <c r="C122" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>1740</v>
+      </c>
+      <c r="B123">
+        <v>34</v>
+      </c>
+      <c r="C123" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>1760</v>
+      </c>
+      <c r="B124">
+        <v>71</v>
+      </c>
+      <c r="C124" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>1770</v>
+      </c>
+      <c r="B125">
+        <v>93</v>
+      </c>
+      <c r="C125" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>1800</v>
+      </c>
+      <c r="B126">
+        <v>75</v>
+      </c>
+      <c r="C126" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>1810</v>
+      </c>
+      <c r="B127">
+        <v>76</v>
+      </c>
+      <c r="C127" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>1830</v>
+      </c>
+      <c r="B128">
+        <v>35</v>
+      </c>
+      <c r="C128" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>1840</v>
+      </c>
+      <c r="B129">
+        <v>77</v>
+      </c>
+      <c r="C129" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>1850</v>
+      </c>
+      <c r="B130">
+        <v>13</v>
+      </c>
+      <c r="C130" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>1860</v>
+      </c>
+      <c r="B131">
+        <v>95</v>
+      </c>
+      <c r="C131" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>1870</v>
+      </c>
+      <c r="B132">
+        <v>96</v>
+      </c>
+      <c r="C132" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>1880</v>
+      </c>
+      <c r="B133">
+        <v>97</v>
+      </c>
+      <c r="C133" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>1890</v>
+      </c>
+      <c r="B134">
+        <v>98</v>
+      </c>
+      <c r="C134" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>1900</v>
+      </c>
+      <c r="B135">
+        <v>78</v>
+      </c>
+      <c r="C135" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>1910</v>
+      </c>
+      <c r="B136">
+        <v>25</v>
+      </c>
+      <c r="C136" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>1920</v>
+      </c>
+      <c r="B137">
+        <v>41</v>
+      </c>
+      <c r="C137" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>1930</v>
+      </c>
+      <c r="B138">
+        <v>53</v>
+      </c>
+      <c r="C138" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>1940</v>
+      </c>
+      <c r="B139">
+        <v>101</v>
+      </c>
+      <c r="C139" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>1950</v>
+      </c>
+      <c r="B140">
+        <v>91</v>
+      </c>
+      <c r="C140" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>1960</v>
+      </c>
+      <c r="B141">
+        <v>79</v>
+      </c>
+      <c r="C141" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>1980</v>
+      </c>
+      <c r="B142">
+        <v>81</v>
+      </c>
+      <c r="C142" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>1990</v>
+      </c>
+      <c r="B143">
+        <v>80</v>
+      </c>
+      <c r="C143" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>2000</v>
+      </c>
+      <c r="B144">
+        <v>92</v>
+      </c>
+      <c r="C144" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>2010</v>
+      </c>
+      <c r="B145">
+        <v>36</v>
+      </c>
+      <c r="C145" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>2020</v>
+      </c>
+      <c r="B146">
+        <v>37</v>
+      </c>
+      <c r="C146" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>2110</v>
+      </c>
+      <c r="B147">
+        <v>121</v>
+      </c>
+      <c r="C147" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>3141</v>
+      </c>
+      <c r="B148">
+        <v>131</v>
+      </c>
+      <c r="C148" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>3143</v>
+      </c>
+      <c r="B149">
+        <v>133</v>
+      </c>
+      <c r="C149" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>9999</v>
+      </c>
+      <c r="B150">
+        <v>999</v>
+      </c>
+      <c r="C150" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:M117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1154,8 +3317,8 @@
     <col min="25" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +3334,7 @@
       <c r="I2" s="42"/>
       <c r="J2" s="42"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1182,139 +3345,178 @@
       <c r="F3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
       <c r="I3" s="8"/>
       <c r="J3" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" s="10" t="s">
-        <v>8</v>
+        <v>234</v>
       </c>
       <c r="D4" s="11"/>
       <c r="F4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="10"/>
+        <v>104</v>
+      </c>
+      <c r="G4" s="45"/>
+      <c r="H4" s="44"/>
       <c r="I4" s="11"/>
-      <c r="J4" s="9">
+      <c r="J4" s="46">
         <v>145</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L4" s="1">
+        <f>VLOOKUP(J4,Temp!$A$2:$C$150,2, FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f>VLOOKUP(J4,Temp!$A$2:$C$150,3, FALSE)</f>
+        <v>Hep A, pediatric, unspecified formulation</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="10">
-        <v>1170</v>
+        <v>52</v>
       </c>
       <c r="D5" s="11"/>
       <c r="F5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="10"/>
+        <v>9</v>
+      </c>
+      <c r="G5" s="45"/>
+      <c r="H5" s="44"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="9">
+      <c r="J5" s="46">
         <v>1170</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L5" s="1">
+        <f>VLOOKUP(J5,Temp!$A$2:$C$150,2, FALSE)</f>
+        <v>52</v>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f>VLOOKUP(J5,Temp!$A$2:$C$150,3, FALSE)</f>
+        <v>Hep A, adult</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="10">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="D6" s="11"/>
       <c r="F6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="10"/>
+        <v>11</v>
+      </c>
+      <c r="G6" s="45"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="11"/>
-      <c r="J6" s="9">
+      <c r="J6" s="46">
         <v>1180</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L6" s="1">
+        <f>VLOOKUP(J6,Temp!$A$2:$C$150,2, FALSE)</f>
+        <v>83</v>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f>VLOOKUP(J6,Temp!$A$2:$C$150,3, FALSE)</f>
+        <v>Hep A, ped/adol, 2 dose</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C7" s="10">
         <v>-145</v>
       </c>
       <c r="D7" s="11"/>
       <c r="F7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="10"/>
+        <v>12</v>
+      </c>
+      <c r="G7" s="45"/>
+      <c r="H7" s="44"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="9">
+      <c r="J7" s="46">
         <v>1190</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L7" s="1">
+        <f>VLOOKUP(J7,Temp!$A$2:$C$150,2, FALSE)</f>
+        <v>84</v>
+      </c>
+      <c r="M7" s="1" t="str">
+        <f>VLOOKUP(J7,Temp!$A$2:$C$150,3, FALSE)</f>
+        <v>Hep A, ped/adol, 3 dose</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="10"/>
+        <v>105</v>
+      </c>
+      <c r="G8" s="45"/>
+      <c r="H8" s="44"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="9">
+      <c r="J8" s="46">
         <v>1200</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L8" s="1">
+        <v>85</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="10" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G9" s="45"/>
+      <c r="H9" s="44"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="9">
+      <c r="J9" s="46">
         <v>146</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F10" s="10"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="L9" s="1">
+        <f>VLOOKUP(J9,Temp!$A$2:$C$150,2, FALSE)</f>
+        <v>104</v>
+      </c>
+      <c r="M9" s="1" t="str">
+        <f>VLOOKUP(J9,Temp!$A$2:$C$150,3, FALSE)</f>
+        <v>Hep A-Hep B</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
@@ -1372,32 +3574,32 @@
     </row>
     <row r="31" spans="2:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C32" s="15">
         <v>1</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="42" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C33" s="42"/>
       <c r="D33" s="42"/>
@@ -1406,30 +3608,30 @@
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="16"/>
       <c r="C34" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -1437,49 +3639,49 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E38" s="9"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E40" s="9"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="9"/>
@@ -1487,21 +3689,21 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="42" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C43" s="42"/>
       <c r="D43" s="42"/>
@@ -1511,98 +3713,98 @@
         <v>4</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E45" s="19"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="19"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E47" s="19"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E49" s="19"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="19"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C52" s="9">
         <v>1</v>
@@ -1610,7 +3812,7 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C53" s="9">
         <v>1</v>
@@ -1618,19 +3820,19 @@
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D56" s="14"/>
       <c r="E56" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C57" s="15">
         <v>2</v>
@@ -1638,7 +3840,7 @@
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="42" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C58" s="42"/>
       <c r="D58" s="42"/>
@@ -1647,30 +3849,30 @@
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="16"/>
       <c r="C59" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C60" s="9"/>
       <c r="D60" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
@@ -1678,49 +3880,49 @@
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C66" s="18"/>
       <c r="D66" s="9"/>
@@ -1728,7 +3930,7 @@
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="42" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C67" s="42"/>
       <c r="D67" s="42"/>
@@ -1738,98 +3940,98 @@
         <v>4</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B69" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E69" s="19"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B70" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="19"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E71" s="19"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D72" s="9"/>
       <c r="E72" s="19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E73" s="19"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="19"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B75" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D75" s="9"/>
       <c r="E75" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C76" s="9">
         <v>1</v>
@@ -1837,7 +4039,7 @@
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B77" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C77" s="9">
         <v>2</v>
@@ -1845,21 +4047,21 @@
     </row>
     <row r="80" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B80" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B81" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C81" s="15">
         <v>2</v>
@@ -1868,7 +4070,7 @@
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B82" s="42" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C82" s="42"/>
       <c r="D82" s="42"/>
@@ -1877,30 +4079,30 @@
     <row r="83" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B83" s="16"/>
       <c r="C83" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B84" s="17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C84" s="9"/>
       <c r="D84" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B85" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
@@ -1908,49 +4110,49 @@
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B86" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C86" s="9"/>
       <c r="D86" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E86" s="9"/>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B87" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C87" s="9"/>
       <c r="D87" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E87" s="9"/>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B88" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B89" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C89" s="18"/>
       <c r="D89" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B90" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C90" s="18"/>
       <c r="D90" s="9"/>
@@ -1958,7 +4160,7 @@
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B91" s="42" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C91" s="42"/>
       <c r="D91" s="42"/>
@@ -1968,60 +4170,60 @@
         <v>4</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B93" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D93" s="9"/>
       <c r="E93" s="19"/>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B94" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D94" s="9"/>
       <c r="E94" s="19"/>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B95" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D95" s="9"/>
       <c r="E95" s="19"/>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B96" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D96" s="9"/>
       <c r="E96" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B97" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C97" s="9">
         <v>2</v>
@@ -2029,7 +4231,7 @@
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B98" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C98" s="9">
         <v>2</v>
@@ -2037,19 +4239,19 @@
     </row>
     <row r="100" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B100" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B101" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C101" s="15">
         <v>3</v>
@@ -2057,7 +4259,7 @@
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B102" s="42" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C102" s="42"/>
       <c r="D102" s="42"/>
@@ -2066,30 +4268,30 @@
     <row r="103" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B103" s="16"/>
       <c r="C103" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B104" s="17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C104" s="9"/>
       <c r="D104" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B105" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C105" s="9"/>
       <c r="D105" s="9"/>
@@ -2097,49 +4299,49 @@
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B106" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C106" s="9"/>
       <c r="D106" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E106" s="9"/>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B107" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C107" s="9"/>
       <c r="D107" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E107" s="9"/>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B108" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D108" s="9"/>
       <c r="E108" s="9"/>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B109" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C109" s="18"/>
       <c r="D109" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B110" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C110" s="18"/>
       <c r="D110" s="9"/>
@@ -2147,7 +4349,7 @@
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B111" s="42" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C111" s="42"/>
       <c r="D111" s="42"/>
@@ -2157,50 +4359,50 @@
         <v>4</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B113" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D113" s="9"/>
       <c r="E113" s="19"/>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B114" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D114" s="9"/>
       <c r="E114" s="19"/>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B115" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D115" s="9"/>
       <c r="E115" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B116" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C116" s="9">
         <v>3</v>
@@ -2208,7 +4410,7 @@
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B117" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C117" s="9">
         <v>2</v>
@@ -2242,8 +4444,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2265,19 +4467,19 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Child" vaccineIds="145, 1180, 1190, 1200"/&gt;</v>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Child" vaccineIds="31, 83, 84, 85"/&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B5&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C5&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Adult" vaccineIds="1170"/&gt;</v>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Adult" vaccineIds="52"/&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Twinrix" vaccineIds="146"/&gt;</v>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Twinrix" vaccineIds="104"/&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
@@ -2675,8 +4877,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2703,54 +4905,54 @@
   <sheetData>
     <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C2" s="42" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="42"/>
       <c r="E2" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="N2" s="17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="27"/>
@@ -2758,7 +4960,7 @@
         <v>38626</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H3" s="4">
         <v>1</v>
@@ -2776,7 +4978,7 @@
         <v>93412</v>
       </c>
       <c r="N3" s="30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O3" s="31">
         <v>39547</v>
@@ -2788,20 +4990,20 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="12">
+        <v>7</v>
+      </c>
+      <c r="D4" s="12" t="str">
         <f>IF(C4="","",IF(ISNA(VLOOKUP(Test!C4,Schedules!F$4:J$28,5)),"? ? ?",VLOOKUP(Test!C4,Schedules!F$4:J$28,5)))</f>
-        <v>145</v>
+        <v>? ? ?</v>
       </c>
       <c r="E4" s="34">
         <v>39052</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
@@ -2820,32 +5022,32 @@
         <v>93412</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O4" s="31">
         <v>39547</v>
       </c>
       <c r="P4" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>testF("Dose 1", "12/01/2006",145, "P2", "2",  "06/01/2007",  "06/01/2007",  "04/01/2009",  "10/01/2155");</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="12">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12" t="str">
         <f>IF(C5="","",IF(ISNA(VLOOKUP(Test!C5,Schedules!F$4:J$28,5)),"? ? ?",VLOOKUP(Test!C5,Schedules!F$4:J$28,5)))</f>
-        <v>145</v>
+        <v>? ? ?</v>
       </c>
       <c r="E5" s="34">
         <v>39243</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="34"/>
@@ -2853,14 +5055,14 @@
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
       <c r="N5" s="30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O5" s="31">
         <v>39547</v>
       </c>
       <c r="P5" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>testF("Dose 2", "06/10/2007",145, "COMPLETE", "",  "01/00/1900",  "01/00/1900",  "01/00/1900",  "01/00/1900");</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -3036,7 +5238,7 @@
     </row>
     <row r="15" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="B15" s="24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C15" s="35"/>
       <c r="D15" s="35"/>
@@ -3051,39 +5253,39 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C16" s="42" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="42"/>
       <c r="E16" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K16" s="42" t="s">
         <v>4</v>
       </c>
       <c r="L16" s="42"/>
       <c r="N16" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="P16" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
@@ -3137,7 +5339,7 @@
       </c>
       <c r="E19" s="34"/>
       <c r="G19" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H19" s="9">
         <v>1</v>
@@ -3146,10 +5348,10 @@
         <v>38763</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K19" s="33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L19" s="12">
         <f>IF(K19="","",IF(ISNA(VLOOKUP(Test!K19,Schedules!F$4:J$28,5)),"? ? ?",VLOOKUP(Test!K19,Schedules!F$4:J$28,5)))</f>

</xml_diff>

<commit_message>
LSVF-9 Added minimum age for HepA
</commit_message>
<xml_diff>
--- a/src/main/webapp/schedules/HepA.xlsx
+++ b/src/main/webapp/schedules/HepA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\tch\forecaster\src\main\webapp\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7415EF7A-F89B-4270-BF2F-D2DB13C60E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAD528F-BA40-4504-B6EF-8F54E2F8E1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48684" yWindow="-12792" windowWidth="20436" windowHeight="25320" tabRatio="405" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="405" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="236">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -3301,8 +3301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3867,7 +3867,9 @@
       <c r="B60" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="9"/>
+      <c r="C60" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="D60" s="9" t="s">
         <v>29</v>
       </c>
@@ -4453,7 +4455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection sqref="A1:A68"/>
     </sheetView>
   </sheetViews>
@@ -4616,7 +4618,7 @@
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C60&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D60&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E60&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;valid age="" interval="6 months" grace="4 days"/&gt;</v>
+        <v xml:space="preserve">    &lt;valid age="18 months" interval="6 months" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>